<commit_message>
All Open as of 20121020
</commit_message>
<xml_diff>
--- a/hotDinner.xlsx
+++ b/hotDinner.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1542" uniqueCount="1283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="1316">
   <si>
     <t>Burger &amp;amp; Lobster Farringdon</t>
   </si>
@@ -3863,6 +3863,105 @@
   </si>
   <si>
     <t>4ecb91fff790bc9a814d51f3</t>
+  </si>
+  <si>
+    <t>4eb7a18e82313162702b73b7</t>
+  </si>
+  <si>
+    <t>4ac518dbf964a52013a920e3</t>
+  </si>
+  <si>
+    <t>4ea85765e3003a42bcf12fac</t>
+  </si>
+  <si>
+    <t>4eb0fccc003940a4cd389006</t>
+  </si>
+  <si>
+    <t>4f47ee93e4b01863527fc7dc</t>
+  </si>
+  <si>
+    <t>4ed1348430f81894af49af32</t>
+  </si>
+  <si>
+    <t>4f108084e4b019e990215c3a</t>
+  </si>
+  <si>
+    <t>4e9d32995503b4a7c128d043</t>
+  </si>
+  <si>
+    <t>4f594ff3e4b05b5a09964d46</t>
+  </si>
+  <si>
+    <t>4ea910a7003973c1923a3357</t>
+  </si>
+  <si>
+    <t>4e9b20d4754aab1ca9dc046c</t>
+  </si>
+  <si>
+    <t>4e9ef7867beb438c5e78e20b</t>
+  </si>
+  <si>
+    <t>4e988480d22d4d655ac32ea8</t>
+  </si>
+  <si>
+    <t>4e98368a02d5a3943708d39d</t>
+  </si>
+  <si>
+    <t>4e906b718b81c6df65af25bd</t>
+  </si>
+  <si>
+    <t>4edb9ed930f83fb79e16baa0</t>
+  </si>
+  <si>
+    <t>4ac518dcf964a52044a920e3</t>
+  </si>
+  <si>
+    <t>4e8d88ff0039a26265603f19</t>
+  </si>
+  <si>
+    <t>4e791e988877ce31d210b81e</t>
+  </si>
+  <si>
+    <t>4e7249e9aeb79ea09553f54c</t>
+  </si>
+  <si>
+    <t>4e1ed9ddae60cd553deae5cd</t>
+  </si>
+  <si>
+    <t>4e85ad77e5fab0fb1125fc54</t>
+  </si>
+  <si>
+    <t>4e653257b993678bb7ca6e65</t>
+  </si>
+  <si>
+    <t>4d658fad129d60fc8cb814c2</t>
+  </si>
+  <si>
+    <t>4e569e0b1f6ecd24d016177d</t>
+  </si>
+  <si>
+    <t>4e3a64ff091a8068d7605b05</t>
+  </si>
+  <si>
+    <t>4e578dbfb9935d203cf9b155</t>
+  </si>
+  <si>
+    <t>4e104d56922ec672352e7631</t>
+  </si>
+  <si>
+    <t>4dfce79d45ddebdfeaac268e</t>
+  </si>
+  <si>
+    <t>4e53a7e0d4c05e0079f45971</t>
+  </si>
+  <si>
+    <t>4e14f263d4c0e3d78b28e1e7</t>
+  </si>
+  <si>
+    <t>4e09e7ab1838eb15af1281c9</t>
+  </si>
+  <si>
+    <t>4e272ba47d8b5ea7247b1158</t>
   </si>
 </sst>
 </file>
@@ -4701,8 +4800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="B159" sqref="B159"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8222,6 +8321,9 @@
       <c r="A160" t="s">
         <v>756</v>
       </c>
+      <c r="B160" t="s">
+        <v>1283</v>
+      </c>
       <c r="D160" t="s">
         <v>1</v>
       </c>
@@ -8242,6 +8344,9 @@
       <c r="A161" t="s">
         <v>761</v>
       </c>
+      <c r="B161" t="s">
+        <v>1284</v>
+      </c>
       <c r="D161" t="s">
         <v>1</v>
       </c>
@@ -8262,6 +8367,9 @@
       <c r="A162" t="s">
         <v>766</v>
       </c>
+      <c r="B162" t="s">
+        <v>1285</v>
+      </c>
       <c r="D162" t="s">
         <v>1</v>
       </c>
@@ -8282,6 +8390,9 @@
       <c r="A163" t="s">
         <v>771</v>
       </c>
+      <c r="B163" t="s">
+        <v>1286</v>
+      </c>
       <c r="D163" t="s">
         <v>1</v>
       </c>
@@ -8302,6 +8413,9 @@
       <c r="A164" t="s">
         <v>776</v>
       </c>
+      <c r="B164" t="s">
+        <v>1287</v>
+      </c>
       <c r="D164" t="s">
         <v>1</v>
       </c>
@@ -8322,6 +8436,9 @@
       <c r="A165" t="s">
         <v>781</v>
       </c>
+      <c r="B165" t="s">
+        <v>1288</v>
+      </c>
       <c r="D165" t="s">
         <v>1</v>
       </c>
@@ -8342,6 +8459,9 @@
       <c r="A166" t="s">
         <v>786</v>
       </c>
+      <c r="B166" t="s">
+        <v>1289</v>
+      </c>
       <c r="D166" t="s">
         <v>1</v>
       </c>
@@ -8362,6 +8482,9 @@
       <c r="A167" t="s">
         <v>791</v>
       </c>
+      <c r="B167" t="s">
+        <v>1290</v>
+      </c>
       <c r="D167" t="s">
         <v>1</v>
       </c>
@@ -8382,6 +8505,9 @@
       <c r="A168" t="s">
         <v>796</v>
       </c>
+      <c r="B168" t="s">
+        <v>1291</v>
+      </c>
       <c r="D168" t="s">
         <v>1</v>
       </c>
@@ -8402,6 +8528,9 @@
       <c r="A169" t="s">
         <v>801</v>
       </c>
+      <c r="B169" t="s">
+        <v>1292</v>
+      </c>
       <c r="D169" t="s">
         <v>1</v>
       </c>
@@ -8419,6 +8548,9 @@
       <c r="A170" t="s">
         <v>805</v>
       </c>
+      <c r="B170" t="s">
+        <v>1293</v>
+      </c>
       <c r="D170" t="s">
         <v>1</v>
       </c>
@@ -8439,6 +8571,9 @@
       <c r="A171" t="s">
         <v>810</v>
       </c>
+      <c r="B171" t="s">
+        <v>1294</v>
+      </c>
       <c r="D171" t="s">
         <v>1</v>
       </c>
@@ -8459,6 +8594,9 @@
       <c r="A172" t="s">
         <v>815</v>
       </c>
+      <c r="B172" s="5" t="s">
+        <v>1295</v>
+      </c>
       <c r="D172" t="s">
         <v>1</v>
       </c>
@@ -8479,6 +8617,9 @@
       <c r="A173" t="s">
         <v>820</v>
       </c>
+      <c r="B173" s="5" t="s">
+        <v>1296</v>
+      </c>
       <c r="D173" t="s">
         <v>1</v>
       </c>
@@ -8499,6 +8640,9 @@
       <c r="A174" t="s">
         <v>824</v>
       </c>
+      <c r="B174" s="5" t="s">
+        <v>1297</v>
+      </c>
       <c r="D174" t="s">
         <v>1</v>
       </c>
@@ -8519,6 +8663,9 @@
       <c r="A175" t="s">
         <v>829</v>
       </c>
+      <c r="B175" t="s">
+        <v>1298</v>
+      </c>
       <c r="D175" t="s">
         <v>1</v>
       </c>
@@ -8539,6 +8686,9 @@
       <c r="A176" t="s">
         <v>834</v>
       </c>
+      <c r="B176" t="s">
+        <v>1299</v>
+      </c>
       <c r="D176" t="s">
         <v>1</v>
       </c>
@@ -8559,6 +8709,9 @@
       <c r="A177" t="s">
         <v>839</v>
       </c>
+      <c r="B177" t="s">
+        <v>1300</v>
+      </c>
       <c r="D177" t="s">
         <v>1</v>
       </c>
@@ -8579,6 +8732,9 @@
       <c r="A178" t="s">
         <v>844</v>
       </c>
+      <c r="B178" s="5" t="s">
+        <v>1301</v>
+      </c>
       <c r="D178" t="s">
         <v>1</v>
       </c>
@@ -8599,6 +8755,9 @@
       <c r="A179" t="s">
         <v>849</v>
       </c>
+      <c r="B179" s="5" t="s">
+        <v>1302</v>
+      </c>
       <c r="D179" t="s">
         <v>1</v>
       </c>
@@ -8619,6 +8778,9 @@
       <c r="A180" t="s">
         <v>854</v>
       </c>
+      <c r="B180" t="s">
+        <v>1303</v>
+      </c>
       <c r="D180" t="s">
         <v>1</v>
       </c>
@@ -8639,6 +8801,9 @@
       <c r="A181" t="s">
         <v>859</v>
       </c>
+      <c r="B181" t="s">
+        <v>1304</v>
+      </c>
       <c r="D181" t="s">
         <v>1</v>
       </c>
@@ -8659,6 +8824,9 @@
       <c r="A182" t="s">
         <v>864</v>
       </c>
+      <c r="B182" s="5" t="s">
+        <v>1305</v>
+      </c>
       <c r="D182" t="s">
         <v>1</v>
       </c>
@@ -8679,6 +8847,9 @@
       <c r="A183" t="s">
         <v>869</v>
       </c>
+      <c r="B183" t="s">
+        <v>1306</v>
+      </c>
       <c r="D183" t="s">
         <v>1</v>
       </c>
@@ -8719,6 +8890,9 @@
       <c r="A185" t="s">
         <v>879</v>
       </c>
+      <c r="B185" s="5" t="s">
+        <v>1307</v>
+      </c>
       <c r="D185" t="s">
         <v>1</v>
       </c>
@@ -8739,6 +8913,9 @@
       <c r="A186" t="s">
         <v>884</v>
       </c>
+      <c r="B186" t="s">
+        <v>1308</v>
+      </c>
       <c r="D186" t="s">
         <v>1</v>
       </c>
@@ -8759,6 +8936,9 @@
       <c r="A187" t="s">
         <v>889</v>
       </c>
+      <c r="B187" s="5" t="s">
+        <v>1309</v>
+      </c>
       <c r="D187" t="s">
         <v>1</v>
       </c>
@@ -8779,6 +8959,9 @@
       <c r="A188" t="s">
         <v>894</v>
       </c>
+      <c r="B188" t="s">
+        <v>1310</v>
+      </c>
       <c r="D188" t="s">
         <v>1</v>
       </c>
@@ -8799,6 +8982,9 @@
       <c r="A189" t="s">
         <v>899</v>
       </c>
+      <c r="B189" t="s">
+        <v>1311</v>
+      </c>
       <c r="D189" t="s">
         <v>1</v>
       </c>
@@ -8819,6 +9005,9 @@
       <c r="A190" t="s">
         <v>904</v>
       </c>
+      <c r="B190" t="s">
+        <v>1312</v>
+      </c>
       <c r="D190" t="s">
         <v>1</v>
       </c>
@@ -8879,6 +9068,9 @@
       <c r="A193" t="s">
         <v>919</v>
       </c>
+      <c r="B193" t="s">
+        <v>1313</v>
+      </c>
       <c r="D193" t="s">
         <v>1</v>
       </c>
@@ -8919,6 +9111,9 @@
       <c r="A195" t="s">
         <v>929</v>
       </c>
+      <c r="B195" t="s">
+        <v>1314</v>
+      </c>
       <c r="D195" t="s">
         <v>1</v>
       </c>
@@ -8938,6 +9133,9 @@
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>934</v>
+      </c>
+      <c r="B196" t="s">
+        <v>1315</v>
       </c>
       <c r="D196" t="s">
         <v>1</v>

</xml_diff>